<commit_message>
Añadido fecha y hora en xlsx
</commit_message>
<xml_diff>
--- a/Datos/almacen.xlsx
+++ b/Datos/almacen.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,11 +472,21 @@
           <t>Trabajador</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0001</t>
+          <t>F0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,17 +496,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -516,376 +526,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>0004</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>0004</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1600</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0004</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1600</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>0004</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1600</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>0004</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1600</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Aaro</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Aaron</t>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>18/08/23</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>15:53</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadido buscar por cliente
</commit_message>
<xml_diff>
--- a/Datos/almacen.xlsx
+++ b/Datos/almacen.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,6 +793,130 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>F0006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>A,B</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2,3</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0,0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>24/08/23</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>F0007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>24/08/23</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Añadido menu para opciones
</commit_message>
<xml_diff>
--- a/Datos/almacen.xlsx
+++ b/Datos/almacen.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -917,6 +917,68 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>F0008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>26/08/23</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>20:59</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
añadido multiplicacion por palets
</commit_message>
<xml_diff>
--- a/Datos/almacen.xlsx
+++ b/Datos/almacen.xlsx
@@ -1,102 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>Referencia</t>
-  </si>
-  <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Unidades</t>
-  </si>
-  <si>
-    <t>Embalajes</t>
-  </si>
-  <si>
-    <t>Cantidad Total</t>
-  </si>
-  <si>
-    <t>Palets</t>
-  </si>
-  <si>
-    <t>Calle</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>Altura</t>
-  </si>
-  <si>
-    <t>Trabajador</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Hora</t>
-  </si>
-  <si>
-    <t>F0001</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>30/08/23</t>
-  </si>
-  <si>
-    <t>23:40</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -104,36 +42,85 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,90 +408,384 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Referencia</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Unidades</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Embalajes</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Cantidad Total</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Palets</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Calle</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Altura</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Trabajador</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>F0001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>31/08/23</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>F0003</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>31/08/23</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>F0002</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>400</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>31/08/23</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>F0004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>800</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Aa</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>31/08/23</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>F1000</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Aa</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>31/08/23</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>